<commit_message>
TB-884 Rework investments linking
</commit_message>
<xml_diff>
--- a/jems-ui/e2e/cypress/fixtures/project/exports/partners-budget/TB-369-export-en-de.xlsx
+++ b/jems-ui/e2e/cypress/fixtures/project/exports/partners-budget/TB-369-export-en-de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jems\ems\jems-ui\e2e\cypress\fixtures\project\exports\partners-budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E901F89-92E0-4803-AE7A-08264E2565B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE29EE1-AAF6-4078-9D32-10E1E7C6639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="3045" windowWidth="19890" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="1605" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_budget_00016_haptic ala" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="142">
   <si>
     <t>00016 - haptic alarm - V1.0 - 2022/12/06 - 12:49:11</t>
   </si>
@@ -438,13 +438,29 @@
   </si>
   <si>
     <t>API generated project proposed unit cost description DE</t>
+  </si>
+  <si>
+    <t>I1.3</t>
+  </si>
+  <si>
+    <t>I1.2</t>
+  </si>
+  <si>
+    <t>I1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -562,10 +578,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -577,9 +594,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8884B357-3CEB-40C3-8141-45345B8CE264}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -893,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1819,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,8 +2380,8 @@
       <c r="L8" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="M8" s="5" t="s">
-        <v>42</v>
+      <c r="M8" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>42</v>
@@ -2453,8 +2472,8 @@
       <c r="L9" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>42</v>
+      <c r="M9" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>42</v>
@@ -2545,8 +2564,8 @@
       <c r="L10" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="M10" s="5" t="s">
-        <v>42</v>
+      <c r="M10" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="N10" s="5" t="s">
         <v>42</v>
@@ -2637,8 +2656,8 @@
       <c r="L11" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M11" s="5" t="s">
-        <v>42</v>
+      <c r="M11" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="N11" s="5" t="s">
         <v>42</v>
@@ -2729,8 +2748,8 @@
       <c r="L12" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M12" s="5" t="s">
-        <v>42</v>
+      <c r="M12" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="N12" s="5" t="s">
         <v>42</v>
@@ -2821,8 +2840,8 @@
       <c r="L13" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M13" s="5" t="s">
-        <v>42</v>
+      <c r="M13" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="N13" s="5" t="s">
         <v>42</v>
@@ -2913,8 +2932,8 @@
       <c r="L14" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="M14" s="5" t="s">
-        <v>42</v>
+      <c r="M14" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>42</v>
@@ -3005,8 +3024,8 @@
       <c r="L15" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="M15" s="5" t="s">
-        <v>42</v>
+      <c r="M15" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="N15" s="5" t="s">
         <v>42</v>
@@ -3097,8 +3116,8 @@
       <c r="L16" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="5" t="s">
-        <v>42</v>
+      <c r="M16" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>42</v>

</xml_diff>